<commit_message>
Chỉnh blog thêm, cập nhật thị trường
</commit_message>
<xml_diff>
--- a/test/query_mysql/Flowchart.xlsx
+++ b/test/query_mysql/Flowchart.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\work7\test\query_mysql\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\work7_dev\work7\test\query_mysql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E2C8B4-F526-4F25-8274-28BD43585E5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67F52772-F551-4787-84CF-922779D4494C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5F33F640-1FE4-4C34-87F1-F2A46F8F38D4}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{5F33F640-1FE4-4C34-87F1-F2A46F8F38D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>Index</t>
   </si>
@@ -72,6 +73,69 @@
   </si>
   <si>
     <t>1. Tính toàn ven</t>
+  </si>
+  <si>
+    <t>STT</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Nhập môn lập trình</t>
+  </si>
+  <si>
+    <t>Kỹ thuật lập trình</t>
+  </si>
+  <si>
+    <t>Cấu trúc dữ liệu và giải thuật</t>
+  </si>
+  <si>
+    <t>Lập trình hướng đối tượng</t>
+  </si>
+  <si>
+    <t>Mạng máy tính căn bản</t>
+  </si>
+  <si>
+    <t>Hệ điều hành</t>
+  </si>
+  <si>
+    <t>Cơ sở dữ liệu</t>
+  </si>
+  <si>
+    <t>Trí tuệ nhân tạo</t>
+  </si>
+  <si>
+    <t>Lập trình python</t>
+  </si>
+  <si>
+    <t>An toàn thông tin</t>
+  </si>
+  <si>
+    <t>Lập trình web</t>
+  </si>
+  <si>
+    <t>Công nghệ phần mềm</t>
+  </si>
+  <si>
+    <t>Hệ quản trị cơ sở dữ liệu</t>
+  </si>
+  <si>
+    <t>Bảo mật web</t>
+  </si>
+  <si>
+    <t>Thiết kế phần mềm hướng đối tượng</t>
+  </si>
+  <si>
+    <t>Lập trình di động</t>
+  </si>
+  <si>
+    <t>SUM</t>
+  </si>
+  <si>
+    <t>Thương mại điện tử</t>
+  </si>
+  <si>
+    <t>Điện toán đám mây</t>
   </si>
 </sst>
 </file>
@@ -95,7 +159,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -118,13 +182,53 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,7 +565,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B14118AE-5BF4-486C-A3B2-C080823773F2}">
   <dimension ref="B4:O18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -536,4 +640,206 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2E819DF-57DB-44BD-BF5B-C87C2BAC3A52}">
+  <dimension ref="C4:E26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="24.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C15">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C16">
+        <v>12</v>
+      </c>
+      <c r="D16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <v>13</v>
+      </c>
+      <c r="D17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <v>14</v>
+      </c>
+      <c r="D18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C19">
+        <v>13</v>
+      </c>
+      <c r="D19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C20">
+        <v>14</v>
+      </c>
+      <c r="D20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C21">
+        <v>15</v>
+      </c>
+      <c r="D21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C22">
+        <v>16</v>
+      </c>
+      <c r="D22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C23">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C24">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C26" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="4">
+        <f>SUM(E5:E25)</f>
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>